<commit_message>
added metadata for fvfm
</commit_message>
<xml_diff>
--- a/metadata/rlc_metadata_07122024.xlsx
+++ b/metadata/rlc_metadata_07122024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssdon\OneDrive\Documents\github\coral-leachate-heat\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E510FC-88D2-4537-A98A-E556990FF1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36E9175-EF45-46F3-9543-3322F6E8A51F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4230" yWindow="817" windowWidth="16185" windowHeight="12136" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,186 +54,6 @@
     <t>species</t>
   </si>
   <si>
-    <t>H102H</t>
-  </si>
-  <si>
-    <t>H62L</t>
-  </si>
-  <si>
-    <t>H32L</t>
-  </si>
-  <si>
-    <t>H92H</t>
-  </si>
-  <si>
-    <t>H92L</t>
-  </si>
-  <si>
-    <t>H42L</t>
-  </si>
-  <si>
-    <t>H82H</t>
-  </si>
-  <si>
-    <t>H32H</t>
-  </si>
-  <si>
-    <t>H72H</t>
-  </si>
-  <si>
-    <t>H52L</t>
-  </si>
-  <si>
-    <t>H102L</t>
-  </si>
-  <si>
-    <t>H72C</t>
-  </si>
-  <si>
-    <t>H42H</t>
-  </si>
-  <si>
-    <t>H22L</t>
-  </si>
-  <si>
-    <t>H12L</t>
-  </si>
-  <si>
-    <t>H62C</t>
-  </si>
-  <si>
-    <t>H62H</t>
-  </si>
-  <si>
-    <t>H12H</t>
-  </si>
-  <si>
-    <t>H22H</t>
-  </si>
-  <si>
-    <t>H92C</t>
-  </si>
-  <si>
-    <t>H52H</t>
-  </si>
-  <si>
-    <t>H72L</t>
-  </si>
-  <si>
-    <t>H22C</t>
-  </si>
-  <si>
-    <t>H42C</t>
-  </si>
-  <si>
-    <t>H52C</t>
-  </si>
-  <si>
-    <t>H12C</t>
-  </si>
-  <si>
-    <t>H32C</t>
-  </si>
-  <si>
-    <t>H82L</t>
-  </si>
-  <si>
-    <t>H82C</t>
-  </si>
-  <si>
-    <t>H102C</t>
-  </si>
-  <si>
-    <t>A102C</t>
-  </si>
-  <si>
-    <t>A102H</t>
-  </si>
-  <si>
-    <t>A92H</t>
-  </si>
-  <si>
-    <t>A22H</t>
-  </si>
-  <si>
-    <t>A12H</t>
-  </si>
-  <si>
-    <t>A102L</t>
-  </si>
-  <si>
-    <t>A72H</t>
-  </si>
-  <si>
-    <t>A32C</t>
-  </si>
-  <si>
-    <t>A12C</t>
-  </si>
-  <si>
-    <t>A12L</t>
-  </si>
-  <si>
-    <t>A22L</t>
-  </si>
-  <si>
-    <t>A52L</t>
-  </si>
-  <si>
-    <t>A82L</t>
-  </si>
-  <si>
-    <t>A62C</t>
-  </si>
-  <si>
-    <t>A62H</t>
-  </si>
-  <si>
-    <t>A52H</t>
-  </si>
-  <si>
-    <t>A62L</t>
-  </si>
-  <si>
-    <t>A52C</t>
-  </si>
-  <si>
-    <t>A42H</t>
-  </si>
-  <si>
-    <t>A42L</t>
-  </si>
-  <si>
-    <t>A22C</t>
-  </si>
-  <si>
-    <t>A92L</t>
-  </si>
-  <si>
-    <t>A32L</t>
-  </si>
-  <si>
-    <t>A32H</t>
-  </si>
-  <si>
-    <t>A72L</t>
-  </si>
-  <si>
-    <t>A82C</t>
-  </si>
-  <si>
-    <t>A72C</t>
-  </si>
-  <si>
-    <t>A82H</t>
-  </si>
-  <si>
-    <t>A92C</t>
-  </si>
-  <si>
-    <t>A42C</t>
-  </si>
-  <si>
     <t>Montipora capitata x Symbiodinium spp.</t>
   </si>
   <si>
@@ -250,6 +70,186 @@
   </si>
   <si>
     <t>control</t>
+  </si>
+  <si>
+    <t>H10.2H</t>
+  </si>
+  <si>
+    <t>H6.2L</t>
+  </si>
+  <si>
+    <t>H3.2L</t>
+  </si>
+  <si>
+    <t>H9.2H</t>
+  </si>
+  <si>
+    <t>H9.2L</t>
+  </si>
+  <si>
+    <t>H8.2H</t>
+  </si>
+  <si>
+    <t>H3.2H</t>
+  </si>
+  <si>
+    <t>H7.2H</t>
+  </si>
+  <si>
+    <t>H5.2L</t>
+  </si>
+  <si>
+    <t>H4.2H</t>
+  </si>
+  <si>
+    <t>H4.2L</t>
+  </si>
+  <si>
+    <t>H10.2L</t>
+  </si>
+  <si>
+    <t>H7.2C</t>
+  </si>
+  <si>
+    <t>H2.2L</t>
+  </si>
+  <si>
+    <t>H1.2L</t>
+  </si>
+  <si>
+    <t>H6.2C</t>
+  </si>
+  <si>
+    <t>H6.2H</t>
+  </si>
+  <si>
+    <t>H1.2H</t>
+  </si>
+  <si>
+    <t>H2.2H</t>
+  </si>
+  <si>
+    <t>H9.2C</t>
+  </si>
+  <si>
+    <t>H5.2H</t>
+  </si>
+  <si>
+    <t>H7.2L</t>
+  </si>
+  <si>
+    <t>H2.2C</t>
+  </si>
+  <si>
+    <t>H4.2C</t>
+  </si>
+  <si>
+    <t>H5.2C</t>
+  </si>
+  <si>
+    <t>H1.2C</t>
+  </si>
+  <si>
+    <t>H3.2C</t>
+  </si>
+  <si>
+    <t>H8.2L</t>
+  </si>
+  <si>
+    <t>H8.2C</t>
+  </si>
+  <si>
+    <t>H10.2C</t>
+  </si>
+  <si>
+    <t>A10.2C</t>
+  </si>
+  <si>
+    <t>A10.2H</t>
+  </si>
+  <si>
+    <t>A9.2H</t>
+  </si>
+  <si>
+    <t>A2.2H</t>
+  </si>
+  <si>
+    <t>A1.2H</t>
+  </si>
+  <si>
+    <t>A10.2L</t>
+  </si>
+  <si>
+    <t>A7.2H</t>
+  </si>
+  <si>
+    <t>A3.2C</t>
+  </si>
+  <si>
+    <t>A1.2C</t>
+  </si>
+  <si>
+    <t>A1.2L</t>
+  </si>
+  <si>
+    <t>A2.2L</t>
+  </si>
+  <si>
+    <t>A5.2L</t>
+  </si>
+  <si>
+    <t>A8.2L</t>
+  </si>
+  <si>
+    <t>A6.2C</t>
+  </si>
+  <si>
+    <t>A6.2H</t>
+  </si>
+  <si>
+    <t>A5.2H</t>
+  </si>
+  <si>
+    <t>A6.2L</t>
+  </si>
+  <si>
+    <t>A5.2C</t>
+  </si>
+  <si>
+    <t>A4.2H</t>
+  </si>
+  <si>
+    <t>A4.2L</t>
+  </si>
+  <si>
+    <t>A2.2C</t>
+  </si>
+  <si>
+    <t>A9.2L</t>
+  </si>
+  <si>
+    <t>A3.2L</t>
+  </si>
+  <si>
+    <t>A3.2H</t>
+  </si>
+  <si>
+    <t>A7.2L</t>
+  </si>
+  <si>
+    <t>A8.2C</t>
+  </si>
+  <si>
+    <t>A7.2C</t>
+  </si>
+  <si>
+    <t>A8.2H</t>
+  </si>
+  <si>
+    <t>A9.2C</t>
+  </si>
+  <si>
+    <t>A4.2C</t>
   </si>
 </sst>
 </file>
@@ -571,8 +571,8 @@
   <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N6" sqref="N6"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -617,22 +617,22 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="E2">
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="G2">
         <v>26</v>
       </c>
       <c r="I2" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
@@ -643,22 +643,22 @@
         <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="E3">
         <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="G3">
         <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
@@ -669,22 +669,22 @@
         <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="G4">
         <v>26</v>
       </c>
       <c r="I4" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
@@ -695,22 +695,22 @@
         <v>42</v>
       </c>
       <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5">
-        <v>9</v>
-      </c>
-      <c r="F5" t="s">
-        <v>72</v>
-      </c>
       <c r="G5">
         <v>26</v>
       </c>
       <c r="I5" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
@@ -721,22 +721,22 @@
         <v>55</v>
       </c>
       <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6">
-        <v>9</v>
-      </c>
-      <c r="F6" t="s">
-        <v>73</v>
-      </c>
       <c r="G6">
         <v>26</v>
       </c>
       <c r="I6" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
@@ -747,22 +747,22 @@
         <v>94</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="E7">
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="G7">
         <v>26</v>
       </c>
       <c r="I7" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
@@ -773,22 +773,22 @@
         <v>107</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="E8">
         <v>3</v>
       </c>
       <c r="F8" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="G8">
         <v>26</v>
       </c>
       <c r="I8" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
@@ -799,22 +799,22 @@
         <v>120</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="E9">
         <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="G9">
         <v>26</v>
       </c>
       <c r="I9" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
@@ -825,22 +825,22 @@
         <v>133</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="E10">
         <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="G10">
         <v>26</v>
       </c>
       <c r="I10" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
@@ -851,22 +851,22 @@
         <v>146</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="E11">
         <v>4</v>
       </c>
       <c r="F11" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="G11">
         <v>26</v>
       </c>
       <c r="I11" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
@@ -877,22 +877,22 @@
         <v>160</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="E12">
         <v>4</v>
       </c>
       <c r="F12" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="G12">
         <v>26</v>
       </c>
       <c r="I12" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
@@ -903,22 +903,22 @@
         <v>173</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="E13">
         <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="G13">
         <v>26</v>
       </c>
       <c r="I13" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
@@ -929,22 +929,22 @@
         <v>186</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="E14">
         <v>7</v>
       </c>
       <c r="F14" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="G14">
         <v>26</v>
       </c>
       <c r="I14" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
@@ -955,22 +955,22 @@
         <v>199</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="E15">
         <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="G15">
         <v>26</v>
       </c>
       <c r="I15" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
@@ -981,22 +981,22 @@
         <v>212</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="G16">
         <v>26</v>
       </c>
       <c r="I16" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
@@ -1007,22 +1007,22 @@
         <v>225</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="E17">
         <v>6</v>
       </c>
       <c r="F17" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="G17">
         <v>26</v>
       </c>
       <c r="I17" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.45">
@@ -1033,22 +1033,22 @@
         <v>238</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D18" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="E18">
         <v>6</v>
       </c>
       <c r="F18" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="G18">
         <v>26</v>
       </c>
       <c r="I18" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.45">
@@ -1059,22 +1059,22 @@
         <v>251</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D19" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="G19">
         <v>26</v>
       </c>
       <c r="I19" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.45">
@@ -1085,22 +1085,22 @@
         <v>264</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="E20">
         <v>2</v>
       </c>
       <c r="F20" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="G20">
         <v>26</v>
       </c>
       <c r="I20" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.45">
@@ -1111,22 +1111,22 @@
         <v>292</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="E21">
         <v>9</v>
       </c>
       <c r="F21" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="G21">
         <v>26</v>
       </c>
       <c r="I21" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.45">
@@ -1137,22 +1137,22 @@
         <v>279</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D22" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="E22">
         <v>5</v>
       </c>
       <c r="F22" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="G22">
         <v>26</v>
       </c>
       <c r="I22" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.45">
@@ -1163,22 +1163,22 @@
         <v>305</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="E23">
         <v>7</v>
       </c>
       <c r="F23" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="G23">
         <v>26</v>
       </c>
       <c r="I23" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.45">
@@ -1189,22 +1189,22 @@
         <v>318</v>
       </c>
       <c r="C24" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D24" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="E24">
         <v>2</v>
       </c>
       <c r="F24" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="G24">
         <v>26</v>
       </c>
       <c r="I24" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.45">
@@ -1215,22 +1215,22 @@
         <v>331</v>
       </c>
       <c r="C25" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D25" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="E25">
         <v>4</v>
       </c>
       <c r="F25" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="G25">
         <v>26</v>
       </c>
       <c r="I25" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.45">
@@ -1241,22 +1241,22 @@
         <v>344</v>
       </c>
       <c r="C26" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D26" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="E26">
         <v>5</v>
       </c>
       <c r="F26" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="G26">
         <v>26</v>
       </c>
       <c r="I26" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.45">
@@ -1267,22 +1267,22 @@
         <v>357</v>
       </c>
       <c r="C27" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D27" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="E27">
         <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="G27">
         <v>26</v>
       </c>
       <c r="I27" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.45">
@@ -1293,22 +1293,22 @@
         <v>370</v>
       </c>
       <c r="C28" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D28" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="E28">
         <v>3</v>
       </c>
       <c r="F28" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="G28">
         <v>26</v>
       </c>
       <c r="I28" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.45">
@@ -1319,22 +1319,22 @@
         <v>383</v>
       </c>
       <c r="C29" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D29" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="E29">
         <v>8</v>
       </c>
       <c r="F29" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="G29">
         <v>26</v>
       </c>
       <c r="I29" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.45">
@@ -1345,22 +1345,22 @@
         <v>396</v>
       </c>
       <c r="C30" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D30" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="E30">
         <v>8</v>
       </c>
       <c r="F30" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="G30">
         <v>26</v>
       </c>
       <c r="I30" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.45">
@@ -1371,22 +1371,22 @@
         <v>422</v>
       </c>
       <c r="C31" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D31" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="E31">
         <v>10</v>
       </c>
       <c r="F31" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="G31">
         <v>26</v>
       </c>
       <c r="I31" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.45">
@@ -1397,22 +1397,22 @@
         <v>435</v>
       </c>
       <c r="C32" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D32" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E32">
         <v>10</v>
       </c>
       <c r="F32" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="G32">
         <v>26</v>
       </c>
       <c r="I32" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.45">
@@ -1423,22 +1423,22 @@
         <v>448</v>
       </c>
       <c r="C33" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D33" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E33">
         <v>10</v>
       </c>
       <c r="F33" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="G33">
         <v>26</v>
       </c>
       <c r="I33" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.45">
@@ -1449,22 +1449,22 @@
         <v>461</v>
       </c>
       <c r="C34" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D34" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E34">
         <v>9</v>
       </c>
       <c r="F34" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="G34">
         <v>26</v>
       </c>
       <c r="I34" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.45">
@@ -1475,22 +1475,22 @@
         <v>474</v>
       </c>
       <c r="C35" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D35" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E35">
         <v>2</v>
       </c>
       <c r="F35" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="G35">
         <v>26</v>
       </c>
       <c r="I35" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.45">
@@ -1501,22 +1501,22 @@
         <v>487</v>
       </c>
       <c r="C36" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D36" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E36">
         <v>1</v>
       </c>
       <c r="F36" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="G36">
         <v>26</v>
       </c>
       <c r="I36" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.45">
@@ -1527,22 +1527,22 @@
         <v>500</v>
       </c>
       <c r="C37" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D37" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E37">
         <v>10</v>
       </c>
       <c r="F37" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="G37">
         <v>26</v>
       </c>
       <c r="I37" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.45">
@@ -1553,22 +1553,22 @@
         <v>513</v>
       </c>
       <c r="C38" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="D38" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E38">
         <v>7</v>
       </c>
       <c r="F38" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="G38">
         <v>26</v>
       </c>
       <c r="I38" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.45">
@@ -1579,22 +1579,22 @@
         <v>526</v>
       </c>
       <c r="C39" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="D39" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E39">
         <v>3</v>
       </c>
       <c r="F39" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="G39">
         <v>26</v>
       </c>
       <c r="I39" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.45">
@@ -1605,22 +1605,22 @@
         <v>539</v>
       </c>
       <c r="C40" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D40" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E40">
         <v>1</v>
       </c>
       <c r="F40" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="G40">
         <v>22</v>
       </c>
       <c r="I40" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.45">
@@ -1631,22 +1631,22 @@
         <v>552</v>
       </c>
       <c r="C41" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D41" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E41">
         <v>1</v>
       </c>
       <c r="F41" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="G41">
         <v>26</v>
       </c>
       <c r="I41" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.45">
@@ -1657,22 +1657,22 @@
         <v>565</v>
       </c>
       <c r="C42" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D42" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E42">
         <v>2</v>
       </c>
       <c r="F42" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="G42">
         <v>24</v>
       </c>
       <c r="I42" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.45">
@@ -1683,22 +1683,22 @@
         <v>578</v>
       </c>
       <c r="C43" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D43" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E43">
         <v>5</v>
       </c>
       <c r="F43" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="G43">
         <v>26</v>
       </c>
       <c r="I43" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.45">
@@ -1709,22 +1709,22 @@
         <v>591</v>
       </c>
       <c r="C44" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D44" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E44">
         <v>8</v>
       </c>
       <c r="F44" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="G44">
         <v>26</v>
       </c>
       <c r="I44" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.45">
@@ -1735,22 +1735,22 @@
         <v>604</v>
       </c>
       <c r="C45" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D45" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E45">
         <v>6</v>
       </c>
       <c r="F45" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="G45">
         <v>26</v>
       </c>
       <c r="I45" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.45">
@@ -1761,22 +1761,22 @@
         <v>617</v>
       </c>
       <c r="C46" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D46" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E46">
         <v>6</v>
       </c>
       <c r="F46" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="G46">
         <v>26</v>
       </c>
       <c r="I46" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.45">
@@ -1787,22 +1787,22 @@
         <v>630</v>
       </c>
       <c r="C47" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D47" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E47">
         <v>5</v>
       </c>
       <c r="F47" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="G47">
         <v>26</v>
       </c>
       <c r="I47" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.45">
@@ -1813,22 +1813,22 @@
         <v>643</v>
       </c>
       <c r="C48" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D48" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E48">
         <v>6</v>
       </c>
       <c r="F48" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="G48">
         <v>26</v>
       </c>
       <c r="I48" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.45">
@@ -1839,22 +1839,22 @@
         <v>656</v>
       </c>
       <c r="C49" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D49" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E49">
         <v>5</v>
       </c>
       <c r="F49" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="G49">
         <v>26</v>
       </c>
       <c r="I49" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.45">
@@ -1865,22 +1865,22 @@
         <v>669</v>
       </c>
       <c r="C50" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="D50" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E50">
         <v>4</v>
       </c>
       <c r="F50" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="G50">
         <v>26</v>
       </c>
       <c r="I50" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.45">
@@ -1891,22 +1891,22 @@
         <v>682</v>
       </c>
       <c r="C51" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D51" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E51">
         <v>4</v>
       </c>
       <c r="F51" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="G51">
         <v>26</v>
       </c>
       <c r="I51" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.45">
@@ -1917,22 +1917,22 @@
         <v>695</v>
       </c>
       <c r="C52" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="D52" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E52">
         <v>2</v>
       </c>
       <c r="F52" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="G52">
         <v>26</v>
       </c>
       <c r="I52" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.45">
@@ -1943,22 +1943,22 @@
         <v>708</v>
       </c>
       <c r="C53" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D53" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E53">
         <v>9</v>
       </c>
       <c r="F53" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="G53">
         <v>26</v>
       </c>
       <c r="I53" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.45">
@@ -1969,22 +1969,22 @@
         <v>721</v>
       </c>
       <c r="C54" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D54" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E54">
         <v>3</v>
       </c>
       <c r="F54" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="G54">
         <v>26</v>
       </c>
       <c r="I54" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.45">
@@ -1995,22 +1995,22 @@
         <v>734</v>
       </c>
       <c r="C55" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D55" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E55">
         <v>3</v>
       </c>
       <c r="F55" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="G55">
         <v>26</v>
       </c>
       <c r="I55" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.45">
@@ -2021,22 +2021,22 @@
         <v>747</v>
       </c>
       <c r="C56" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D56" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E56">
         <v>7</v>
       </c>
       <c r="F56" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="G56">
         <v>26</v>
       </c>
       <c r="I56" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.45">
@@ -2047,22 +2047,22 @@
         <v>760</v>
       </c>
       <c r="C57" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D57" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E57">
         <v>8</v>
       </c>
       <c r="F57" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="G57">
         <v>26</v>
       </c>
       <c r="I57" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.45">
@@ -2073,22 +2073,22 @@
         <v>773</v>
       </c>
       <c r="C58" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="D58" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E58">
         <v>7</v>
       </c>
       <c r="F58" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="G58">
         <v>25</v>
       </c>
       <c r="I58" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.45">
@@ -2099,22 +2099,22 @@
         <v>786</v>
       </c>
       <c r="C59" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D59" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E59">
         <v>8</v>
       </c>
       <c r="F59" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="G59">
         <v>26</v>
       </c>
       <c r="I59" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.45">
@@ -2125,22 +2125,22 @@
         <v>799</v>
       </c>
       <c r="C60" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D60" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E60">
         <v>9</v>
       </c>
       <c r="F60" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="G60">
         <v>26</v>
       </c>
       <c r="I60" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.45">
@@ -2151,22 +2151,22 @@
         <v>812</v>
       </c>
       <c r="C61" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D61" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E61">
         <v>4</v>
       </c>
       <c r="F61" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="G61">
         <v>26</v>
       </c>
       <c r="I61" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>